<commit_message>
Adding A data of Foods & Drinks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GLS\Z-Project\07-2025\04-All Websites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46546797-C4BE-4B54-843E-1D8799DA90B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872A72B-FD4D-44ED-AB07-916BB145D93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{28AA069D-6455-47CE-AC51-E6AA5DBC55FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>category</t>
   </si>
@@ -142,6 +142,63 @@
   </si>
   <si>
     <t>https://shimmering-torrone-43b7c4.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-1</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-2</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-3</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-4</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-5</t>
+  </si>
+  <si>
+    <t>https://downgit.github.io/#/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-6</t>
+  </si>
+  <si>
+    <t>https://678f8495f2301b696ef5a20d--spiffy-douhua-5a83ad.netlify.app/</t>
+  </si>
+  <si>
+    <t>food &amp; Drink</t>
+  </si>
+  <si>
+    <t>food-1</t>
+  </si>
+  <si>
+    <t>food-2</t>
+  </si>
+  <si>
+    <t>food-3</t>
+  </si>
+  <si>
+    <t>food-4</t>
+  </si>
+  <si>
+    <t>food-5</t>
+  </si>
+  <si>
+    <t>food-6</t>
+  </si>
+  <si>
+    <t>https://678f84e131b5dc56aef696af--coruscating-moxie-c6f523.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://glistening-fudge-538963.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://678f85617d243971ae9804ed--spectacular-meringue-c25aa7.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://678f859734afd74ec8943e24--helpful-semolina-9a505f.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://678f85c61bfff87ce64882f6--tourmaline-babka-d129eb.netlify.app/</t>
   </si>
 </sst>
 </file>
@@ -510,14 +567,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B312B09-E237-492F-B707-6ABE43B1FABF}">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.08984375" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" customWidth="1"/>
     <col min="5" max="5" width="23.81640625" customWidth="1"/>
@@ -628,6 +686,9 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
       <c r="E8" t="s">
         <v>30</v>
       </c>
@@ -639,6 +700,9 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
       <c r="E9" t="s">
         <v>31</v>
       </c>
@@ -650,6 +714,9 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
@@ -661,6 +728,9 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
       <c r="E11" t="s">
         <v>33</v>
       </c>
@@ -672,6 +742,9 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
@@ -683,8 +756,77 @@
       <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +834,10 @@
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" location="/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Education/Education-4" xr:uid="{460C8933-0983-4806-BBFA-064656DCEB40}"/>
     <hyperlink ref="D7" r:id="rId2" location="/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Education/Education-6" xr:uid="{6B435411-F74E-4FEE-AC5D-906BC7863853}"/>
+    <hyperlink ref="D13" r:id="rId3" location="/home?url=https://github.com/Abrar9825/Websites_ForWebsite/tree/main/Portfolio/port-6" xr:uid="{A2BD50EC-53E6-47B7-9680-16A806047024}"/>
+    <hyperlink ref="E13" r:id="rId4" xr:uid="{C3A62042-15DD-4E21-94D1-25E5358EE5C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>